<commit_message>
Attendance：Date date→String date OfferStatus：int yearMonth→LocalDate date OfferRepository：yearMonth検索→date検索
</commit_message>
<xml_diff>
--- a/3.勤怠管理アプリ/05_内部仕様書/クラス図/クラス図(Attendanceクラス).xlsx
+++ b/3.勤怠管理アプリ/05_内部仕様書/クラス図/クラス図(Attendanceクラス).xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>更新日</t>
     <rPh sb="0" eb="3">
@@ -126,10 +126,6 @@
     <t>//勤怠識別番号</t>
   </si>
   <si>
-    <t>- Date  date</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>//勤務日</t>
     <rPh sb="2" eb="5">
       <t>キンムビ</t>
@@ -304,10 +300,6 @@
     <t>@ManyToOne (FK:apply_id)</t>
   </si>
   <si>
-    <t>@NotNull/@Min(0)/@Max(2400)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>@NotNull/@column(length=10)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -357,6 +349,10 @@
   </si>
   <si>
     <t>- OfferStatus offerStatus</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>- String  date</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -611,46 +607,46 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -730,7 +726,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="変更履歴!$A$1:$E$2" spid="_x0000_s1076"/>
+                  <a14:cameraTool cellRange="変更履歴!$A$1:$E$2" spid="_x0000_s1078"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -1414,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1432,396 +1428,396 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B9" s="7"/>
+      <c r="C9" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B10" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B13" s="7"/>
+      <c r="C13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B15" s="7"/>
+      <c r="C15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="B16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B17" s="7"/>
+      <c r="C17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B9" s="8"/>
-      <c r="C9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B13" s="8"/>
-      <c r="C13" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B14" s="18" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B19" s="7"/>
+      <c r="C19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B20" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B21" s="7"/>
+      <c r="C21" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B22" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B23" s="7"/>
+      <c r="C23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B25" s="7"/>
+      <c r="C25" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B26" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B27" s="7"/>
+      <c r="C27" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B28" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B29" s="7"/>
+      <c r="C29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B31" s="7"/>
+      <c r="C31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B32" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B33" s="7"/>
+      <c r="C33" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B34" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B35" s="7"/>
+      <c r="C35" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B36" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B15" s="8"/>
-      <c r="C15" s="20" t="s">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B37" s="7"/>
+      <c r="C37" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" s="8"/>
-      <c r="C17" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" s="8"/>
-      <c r="C19" s="20" t="s">
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B38" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B21" s="8"/>
-      <c r="C21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B22" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="8"/>
-      <c r="C23" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B24" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B25" s="8"/>
-      <c r="C25" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B26" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B27" s="8"/>
-      <c r="C27" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B28" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B29" s="8"/>
-      <c r="C29" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B30" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="9"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B31" s="8"/>
-      <c r="C31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B32" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B33" s="8"/>
-      <c r="C33" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B34" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B35" s="8"/>
-      <c r="C35" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B36" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B37" s="8"/>
-      <c r="C37" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B38" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B39" s="11"/>
-      <c r="C39" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="13"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>